<commit_message>
Algorithm update (inverse index defaults to all lines and indices with no arguments)
statistics and timing updated
</commit_message>
<xml_diff>
--- a/stats/timings.xlsx
+++ b/stats/timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tyson/Documents/Academic/4th Year/ELEN4020/Labs/Lab3/stats/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868831DA-B565-1B4A-938D-D298962E1768}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C42337C-68D0-9C45-B3E1-7BC2A0440B80}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" xr2:uid="{B2F079D1-0A62-E247-9521-E58C50C3DE37}"/>
+    <workbookView xWindow="3220" yWindow="2640" windowWidth="28040" windowHeight="17440" xr2:uid="{B2F079D1-0A62-E247-9521-E58C50C3DE37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -480,7 +480,7 @@
         <v>154.75899999999999</v>
       </c>
       <c r="G2">
-        <v>176.88200000000001</v>
+        <v>208.34899999999999</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -503,7 +503,7 @@
         <v>146.46700000000001</v>
       </c>
       <c r="G3">
-        <v>500.26400000000001</v>
+        <v>472.58300000000003</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -526,7 +526,7 @@
         <v>164.75899999999999</v>
       </c>
       <c r="G4">
-        <v>799.88699999999994</v>
+        <v>777.02700000000004</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -549,7 +549,7 @@
         <v>154.376</v>
       </c>
       <c r="G5">
-        <v>1419.1420000000001</v>
+        <v>1201.2919999999999</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -572,7 +572,7 @@
         <v>146.87899999999999</v>
       </c>
       <c r="G6">
-        <v>1609.441</v>
+        <v>1540.7560000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -595,7 +595,7 @@
         <v>133.62700000000001</v>
       </c>
       <c r="G7">
-        <v>10169.58</v>
+        <v>8420.9240000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>